<commit_message>
Update project report and presentation
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6800" activeTab="2"/>
+    <workbookView windowWidth="18350" windowHeight="8010" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="GPT-4.1-mini" sheetId="1" r:id="rId1"/>
+    <sheet name="GPT-4.1-mini" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="MedGemma 4B" sheetId="2" r:id="rId2"/>
     <sheet name="MedGemma 4B DPO" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -151,31 +151,31 @@
     <t>Điểm trung bình</t>
   </si>
   <si>
-    <t>logs\medgemma-4b-it-2025_07_20-02_34.txt</t>
+    <t>logs\medgemma-4b-dpo-2025_07_20-02_34.txt</t>
   </si>
   <si>
     <t>tức ngực, khó thở nhẹ khoảng 2-3 ngày có lúc ớn lạnh, mất vị giác, không ho, không sốt, không sổ mũi, không đau họng, không mệt mỏi</t>
   </si>
   <si>
-    <t>logs\medgemma-4b-it-2025_07_20-02_46.txt</t>
-  </si>
-  <si>
-    <t>logs\medgemma-4b-it-2025_07_20-22_52.txt</t>
-  </si>
-  <si>
-    <t>logs\medgemma-4b-it-2025_07_20-23_05.txt</t>
+    <t>logs\medgemma-4b-dpo-2025_07_20-02_46.txt</t>
+  </si>
+  <si>
+    <t>logs\medgemma-4b-dpo-2025_07_20-22_52.txt</t>
+  </si>
+  <si>
+    <t>logs\medgemma-4b-dpo-2025_07_20-23_05.txt</t>
   </si>
   <si>
     <t>Đau tức ngực khi đi cầu thang hoặc làm việc nặng, tim đập nhanh hơn bình thường trong 1 tuần gần đây</t>
   </si>
   <si>
-    <t>logs\medgemma-4b-it-2025_07_21-01_36.txt</t>
+    <t>logs\medgemma-4b-dpo-2025_07_21-01_36.txt</t>
   </si>
   <si>
     <t>đau ngực, mệt mỏi, buồn ngủ ban ngày, đôi khi khó thở khi nằm xuống, không bị đau ngực liên tục, không có tiền sử bệnh tim hoặc phổi, không hút thuốc</t>
   </si>
   <si>
-    <t>logs\medgemma-4b-it-2025_07_21-01_42.txt</t>
+    <t>logs\medgemma-4b-dpo-2025_07_21-01_42.txt</t>
   </si>
   <si>
     <t>chóng mặt mức độ vừa, hay nhức đầu, chảy máu cam không rõ lý do, không bị đau nửa đầu, buồn nôn hay mờ mắt, hiện tại không dùng thuốc nào</t>
@@ -187,19 +187,19 @@
     <t>mờ mắt, hoa mắt khi đứng dậy, nhức đầu, đôi lúc buồn nôn nhẹ, mệt mỏi liên tục, hiện tại tôi chưa dùng thuốc điều trị</t>
   </si>
   <si>
-    <t>logs\medgemma-4b-it-2025_07_21-02_59.txt</t>
+    <t>logs\medgemma-4b-dpo-2025_07_21-02_59.txt</t>
   </si>
   <si>
     <t>dễ lo lắng, mệt mỏi, kém tập trung, thường xuyên mất ngủ trong khoảng 2 tuần gần đây, làm gì cũng không có tinh thần</t>
   </si>
   <si>
-    <t>logs\medgemma-4b-it-2025_07_21-03_29.txt</t>
+    <t>logs\medgemma-4b-dpo-2025_07_21-03_29.txt</t>
   </si>
   <si>
     <t>buồn bã, ít nói chuyện hơn, không còn hứng thú với công việc từng yêu thích, không có thay đổi quá lớn trong cuộc sống, cảm thấy cô đơn và lạc lõng, tự đánh giá tiêu cực</t>
   </si>
   <si>
-    <t>logs\medgemma-4b-it-2025_07_21-03_50.txt</t>
+    <t>logs\medgemma-4b-dpo-2025_07_21-03_50.txt</t>
   </si>
 </sst>
 </file>
@@ -1423,7 +1423,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="A12" sqref="$A12:$XFD16"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14.5"/>
@@ -1637,10 +1637,10 @@
   <sheetPr/>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14.5"/>
@@ -2091,35 +2091,35 @@
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="9">
-        <f>AVERAGE(D2:D11)</f>
+        <f t="shared" ref="D12:K12" si="1">AVERAGE(D2:D11)</f>
         <v>1</v>
       </c>
       <c r="E12" s="9">
-        <f>AVERAGE(E2:E11)</f>
+        <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
       <c r="F12" s="9">
-        <f>AVERAGE(F2:F11)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G12" s="9">
-        <f>AVERAGE(G2:G11)</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="H12" s="9">
-        <f>AVERAGE(H2:H11)</f>
+        <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
       <c r="I12" s="9">
-        <f>AVERAGE(I2:I11)</f>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="J12" s="9">
-        <f>AVERAGE(J2:J11)</f>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="K12" s="9">
-        <f>AVERAGE(K2:K11)</f>
+        <f t="shared" si="1"/>
         <v>2.2</v>
       </c>
       <c r="L12" s="11"/>
@@ -2138,10 +2138,10 @@
   <sheetPr/>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14.5"/>
@@ -2410,7 +2410,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H7" s="5">
         <v>1</v>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="K7" s="10">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>48</v>
@@ -2605,7 +2605,7 @@
       </c>
       <c r="G12" s="9">
         <f t="shared" si="1"/>
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="H12" s="9">
         <f t="shared" si="1"/>
@@ -2621,7 +2621,7 @@
       </c>
       <c r="K12" s="9">
         <f t="shared" si="1"/>
-        <v>4.25</v>
+        <v>4.3</v>
       </c>
       <c r="L12" s="11"/>
     </row>

</xml_diff>